<commit_message>
Updated with Azure API Key
</commit_message>
<xml_diff>
--- a/automation_testing.xlsx
+++ b/automation_testing.xlsx
@@ -1080,12 +1080,12 @@
       </c>
       <c r="E15" s="16" t="inlineStr">
         <is>
-          <t>RETURNS</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F15" s="17" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="G15" s="18" t="n"/>

</xml_diff>

<commit_message>
Commit After Adding ChromaDB and Adding Examples -10/25
</commit_message>
<xml_diff>
--- a/automation_testing.xlsx
+++ b/automation_testing.xlsx
@@ -940,12 +940,12 @@
       </c>
       <c r="E14" s="16" t="inlineStr">
         <is>
-          <t>OTHERS</t>
+          <t>Returns</t>
         </is>
       </c>
       <c r="F14" s="17" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
       <c r="G14" s="17" t="n"/>
@@ -1552,12 +1552,12 @@
       </c>
       <c r="E32" s="16" t="inlineStr">
         <is>
-          <t>DAMAGES</t>
+          <t>OTHERS</t>
         </is>
       </c>
       <c r="F32" s="16" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="E70" s="0" t="inlineStr">
         <is>
-          <t>Returns</t>
+          <t>RETURNS</t>
         </is>
       </c>
       <c r="F70" s="0" t="inlineStr">

</xml_diff>